<commit_message>
Excel Reader test added
</commit_message>
<xml_diff>
--- a/SantanderBank/src/test/java/dataFeatures/Book1.xlsx
+++ b/SantanderBank/src/test/java/dataFeatures/Book1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manir\Desktop\GroupProject\Group-13\SantanderBank\src\test\java\dataDrivenExcel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manir\Desktop\GroupProject\Group-13\SantanderBank\src\test\java\dataFeatures\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,44 +24,37 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>User</t>
+    <t>Product</t>
   </si>
   <si>
-    <t>Password</t>
+    <t>Business Loan</t>
   </si>
   <si>
-    <t>Maniruzzaman</t>
+    <t>Car Loan</t>
   </si>
   <si>
-    <t>test1234</t>
+    <t>Home Loan</t>
   </si>
   <si>
-    <t>NurulIslam</t>
-  </si>
-  <si>
-    <t>test1235</t>
-  </si>
-  <si>
-    <t>LobidChodhury</t>
-  </si>
-  <si>
-    <t>test1236</t>
-  </si>
-  <si>
-    <t>ImranKhan</t>
-  </si>
-  <si>
-    <t>test1237</t>
+    <t>Student Loan</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -89,8 +82,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -371,59 +365,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>